<commit_message>
Teams Marty, Brian, and Kevin added
</commit_message>
<xml_diff>
--- a/data/food_drink_trivia_results.xlsx
+++ b/data/food_drink_trivia_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/Trivia/food_drink_trivia/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDA9F05-F1A8-AD4C-9A03-7C8D197C4AE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A366FC03-4C8D-144A-9E77-1ABB25ADAB04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15760" xr2:uid="{283CCA2A-C3D6-8F49-8CBB-1552C6AB69C2}"/>
   </bookViews>
@@ -438,7 +438,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.83203125" defaultRowHeight="16"/>
@@ -477,31 +477,31 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1.5</v>
+        <v>5.5</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>3.5</v>
       </c>
       <c r="D2">
         <f>B2+C2</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E2">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="F2">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="H2">
         <f>F2+G2</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I2">
         <f>D2+E2+H2</f>
-        <v>10</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -509,31 +509,31 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D8" si="0">B3+C3</f>
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <v>5</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>4.5</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H8" si="1">F3+G3</f>
-        <v>2.5</v>
+        <v>8</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I8" si="2">D3+E3+H3</f>
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -541,10 +541,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
@@ -573,31 +573,31 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="C5">
         <v>1.5</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
         <v>3.5</v>
       </c>
-      <c r="E5">
-        <v>8</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
       <c r="G5">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="I5">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="6" spans="1:9">

</xml_diff>

<commit_message>
Team Brian correction and team Noonan added
</commit_message>
<xml_diff>
--- a/data/food_drink_trivia_results.xlsx
+++ b/data/food_drink_trivia_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/Trivia/food_drink_trivia/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A366FC03-4C8D-144A-9E77-1ABB25ADAB04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3B2790-1578-0545-B60F-A62186B0B730}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15760" xr2:uid="{283CCA2A-C3D6-8F49-8CBB-1552C6AB69C2}"/>
   </bookViews>
@@ -438,7 +438,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.83203125" defaultRowHeight="16"/>
@@ -519,7 +519,7 @@
         <v>6</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3">
         <v>4.5</v>
@@ -533,7 +533,7 @@
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I8" si="2">D3+E3+H3</f>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -669,31 +669,31 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
       <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>3.5</v>
+      </c>
+      <c r="G8">
         <v>4</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
-        <v>1.5</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>3.5</v>
+        <v>7.5</v>
       </c>
       <c r="I8">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>